<commit_message>
size of plot bigger
</commit_message>
<xml_diff>
--- a/santa_clara_county/CFR_in_LTCF_version2.xlsx
+++ b/santa_clara_county/CFR_in_LTCF_version2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stk\Documents\GitHub\covid\santa_clara_county\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E136CF76-D309-455E-A1F8-486FAF0CECDD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABE35164-1B8D-44D7-89DD-E10F7833BDA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3840" yWindow="7875" windowWidth="20295" windowHeight="15435" xr2:uid="{117AAEEC-A907-4519-B809-3E58232F1605}"/>
+    <workbookView xWindow="5205" yWindow="1230" windowWidth="20295" windowHeight="15435" firstSheet="1" activeTab="2" xr2:uid="{117AAEEC-A907-4519-B809-3E58232F1605}"/>
   </bookViews>
   <sheets>
     <sheet name="Count_of_deaths_with_COVID-19_b" sheetId="3" r:id="rId1"/>
@@ -20,8 +20,8 @@
   </sheets>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="3" r:id="rId5"/>
-    <pivotCache cacheId="10" r:id="rId6"/>
+    <pivotCache cacheId="0" r:id="rId5"/>
+    <pivotCache cacheId="1" r:id="rId6"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -213,7 +213,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
@@ -228,7 +228,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
@@ -3138,16 +3137,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>533400</xdr:colOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>314325</xdr:colOff>
       <xdr:row>11</xdr:row>
       <xdr:rowOff>52387</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>18</xdr:col>
       <xdr:colOff>228600</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>128587</xdr:rowOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -10048,7 +10047,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{180C8EF8-D1EF-4BCE-AB42-D4EA978E5D89}" name="PivotTable1" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{180C8EF8-D1EF-4BCE-AB42-D4EA978E5D89}" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="J4:K21" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="5">
     <pivotField axis="axisRow" numFmtId="14" showAll="0">
@@ -11069,7 +11068,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{31664277-CDE3-4028-B339-8FD041FB6786}" name="PivotTable2" cacheId="10" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{31664277-CDE3-4028-B339-8FD041FB6786}" name="PivotTable2" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="J4:K13" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="6">
     <pivotField dataField="1" showAll="0"/>
@@ -11548,7 +11547,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{F4B67D5F-7A9E-4B50-9A85-8B343C30AFB7}" name="PivotTable4" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{F4B67D5F-7A9E-4B50-9A85-8B343C30AFB7}" name="PivotTable4" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="D1:E18" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="5">
     <pivotField axis="axisRow" numFmtId="14" showAll="0">
@@ -12569,7 +12568,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{362FE6F2-7317-416C-9596-75ED72BF6453}" name="PivotTable3" cacheId="10" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{362FE6F2-7317-416C-9596-75ED72BF6453}" name="PivotTable3" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A1:B10" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="6">
     <pivotField dataField="1" showAll="0"/>
@@ -13366,8 +13365,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66CC7010-71E4-4BF0-BBA5-372253FABEA9}">
   <dimension ref="A1:K894"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A208" workbookViewId="0">
-      <selection activeCell="I37" sqref="I37"/>
+    <sheetView topLeftCell="A208" workbookViewId="0">
+      <selection activeCell="K210" sqref="K210"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13516,7 +13515,7 @@
       <c r="J5" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="K5" s="8">
+      <c r="K5">
         <v>543</v>
       </c>
     </row>
@@ -13544,10 +13543,10 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="J6" s="9" t="s">
+      <c r="J6" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="K6" s="8">
+      <c r="K6">
         <v>7</v>
       </c>
     </row>
@@ -13575,10 +13574,10 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="J7" s="9" t="s">
+      <c r="J7" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="K7" s="8">
+      <c r="K7">
         <v>65</v>
       </c>
     </row>
@@ -13606,10 +13605,10 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="J8" s="9" t="s">
+      <c r="J8" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="K8" s="8">
+      <c r="K8">
         <v>62</v>
       </c>
     </row>
@@ -13637,10 +13636,10 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="J9" s="9" t="s">
+      <c r="J9" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="K9" s="8">
+      <c r="K9">
         <v>409</v>
       </c>
     </row>
@@ -13671,7 +13670,7 @@
       <c r="J10" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="K10" s="8">
+      <c r="K10">
         <v>286</v>
       </c>
     </row>
@@ -13699,10 +13698,10 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="J11" s="9" t="s">
+      <c r="J11" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="K11" s="8">
+      <c r="K11">
         <v>244</v>
       </c>
     </row>
@@ -13730,10 +13729,10 @@
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="J12" s="9" t="s">
+      <c r="J12" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="K12" s="8">
+      <c r="K12">
         <v>10</v>
       </c>
     </row>
@@ -13761,10 +13760,10 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="J13" s="9" t="s">
+      <c r="J13" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="K13" s="8">
+      <c r="K13">
         <v>17</v>
       </c>
     </row>
@@ -13792,10 +13791,10 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="J14" s="9" t="s">
+      <c r="J14" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="K14" s="8">
+      <c r="K14">
         <v>15</v>
       </c>
     </row>
@@ -13826,7 +13825,7 @@
       <c r="J15" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="K15" s="8">
+      <c r="K15">
         <v>125</v>
       </c>
     </row>
@@ -13854,10 +13853,10 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="J16" s="9" t="s">
+      <c r="J16" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="K16" s="8">
+      <c r="K16">
         <v>57</v>
       </c>
     </row>
@@ -13885,10 +13884,10 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="J17" s="9" t="s">
+      <c r="J17" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="K17" s="8">
+      <c r="K17">
         <v>28</v>
       </c>
     </row>
@@ -13916,10 +13915,10 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="J18" s="9" t="s">
+      <c r="J18" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="K18" s="8">
+      <c r="K18">
         <v>25</v>
       </c>
     </row>
@@ -13947,10 +13946,10 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="J19" s="9" t="s">
+      <c r="J19" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="K19" s="8">
+      <c r="K19">
         <v>15</v>
       </c>
     </row>
@@ -13981,7 +13980,7 @@
       <c r="J20" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="K20" s="8">
+      <c r="K20">
         <v>9</v>
       </c>
     </row>
@@ -14012,7 +14011,7 @@
       <c r="J21" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="K21" s="8">
+      <c r="K21">
         <v>963</v>
       </c>
     </row>
@@ -35924,7 +35923,7 @@
       <c r="J5" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="K5" s="8">
+      <c r="K5">
         <v>5349</v>
       </c>
     </row>
@@ -35938,10 +35937,10 @@
       <c r="C6" s="4">
         <v>43898</v>
       </c>
-      <c r="J6" s="9" t="s">
+      <c r="J6" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="K6" s="8">
+      <c r="K6">
         <v>101</v>
       </c>
     </row>
@@ -35955,10 +35954,10 @@
       <c r="C7" s="4">
         <v>43899</v>
       </c>
-      <c r="J7" s="9" t="s">
+      <c r="J7" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="K7" s="8">
+      <c r="K7">
         <v>779</v>
       </c>
     </row>
@@ -35972,10 +35971,10 @@
       <c r="C8" s="4">
         <v>43900</v>
       </c>
-      <c r="J8" s="9" t="s">
+      <c r="J8" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="K8" s="8">
+      <c r="K8">
         <v>720</v>
       </c>
     </row>
@@ -35989,10 +35988,10 @@
       <c r="C9" s="4">
         <v>43901</v>
       </c>
-      <c r="J9" s="9" t="s">
+      <c r="J9" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="K9" s="8">
+      <c r="K9">
         <v>3749</v>
       </c>
     </row>
@@ -36009,7 +36008,7 @@
       <c r="J10" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="K10" s="8">
+      <c r="K10">
         <v>1044</v>
       </c>
     </row>
@@ -36023,10 +36022,10 @@
       <c r="C11" s="4">
         <v>43903</v>
       </c>
-      <c r="J11" s="9" t="s">
+      <c r="J11" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="K11" s="8">
+      <c r="K11">
         <v>1020</v>
       </c>
     </row>
@@ -36040,10 +36039,10 @@
       <c r="C12" s="4">
         <v>43904</v>
       </c>
-      <c r="J12" s="9" t="s">
+      <c r="J12" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="K12" s="8">
+      <c r="K12">
         <v>24</v>
       </c>
     </row>
@@ -36060,7 +36059,7 @@
       <c r="J13" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="K13" s="8">
+      <c r="K13">
         <v>6393</v>
       </c>
     </row>
@@ -40078,8 +40077,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1EFB7F1A-0D0B-48B0-BFA1-BCFFB561B227}">
   <dimension ref="A1:M18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H23" sqref="H23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="T18" sqref="T18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -40114,23 +40113,23 @@
       <c r="A2" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="B2" s="8">
+      <c r="B2">
         <v>5349</v>
       </c>
       <c r="D2" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="E2" s="8">
+      <c r="E2">
         <v>543</v>
       </c>
-      <c r="I2" s="10" t="s">
+      <c r="I2" s="9" t="s">
         <v>15</v>
       </c>
       <c r="J2">
         <f>$E2/$B2</f>
         <v>0.10151430173864273</v>
       </c>
-      <c r="L2" s="11" t="s">
+      <c r="L2" s="10" t="s">
         <v>27</v>
       </c>
       <c r="M2">
@@ -40138,26 +40137,26 @@
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A3" s="9" t="s">
+      <c r="A3" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="B3" s="8">
+      <c r="B3">
         <v>101</v>
       </c>
-      <c r="D3" s="9" t="s">
+      <c r="D3" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="E3" s="8">
+      <c r="E3">
         <v>7</v>
       </c>
-      <c r="I3" s="11" t="s">
+      <c r="I3" s="10" t="s">
         <v>20</v>
       </c>
       <c r="J3">
         <f t="shared" ref="J3:J9" si="0">$E3/$B3</f>
         <v>6.9306930693069313E-2</v>
       </c>
-      <c r="L3" s="11" t="s">
+      <c r="L3" s="10" t="s">
         <v>28</v>
       </c>
       <c r="M3">
@@ -40165,26 +40164,26 @@
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A4" s="9" t="s">
+      <c r="A4" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="B4" s="8">
+      <c r="B4">
         <v>779</v>
       </c>
-      <c r="D4" s="9" t="s">
+      <c r="D4" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="E4" s="8">
+      <c r="E4">
         <v>65</v>
       </c>
-      <c r="I4" s="11" t="s">
+      <c r="I4" s="10" t="s">
         <v>21</v>
       </c>
       <c r="J4">
         <f t="shared" si="0"/>
         <v>8.3440308087291401E-2</v>
       </c>
-      <c r="L4" s="11" t="s">
+      <c r="L4" s="10" t="s">
         <v>29</v>
       </c>
       <c r="M4">
@@ -40192,26 +40191,26 @@
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A5" s="9" t="s">
+      <c r="A5" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="B5" s="8">
+      <c r="B5">
         <v>720</v>
       </c>
-      <c r="D5" s="9" t="s">
+      <c r="D5" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="E5" s="8">
+      <c r="E5">
         <v>62</v>
       </c>
-      <c r="I5" s="11" t="s">
+      <c r="I5" s="10" t="s">
         <v>22</v>
       </c>
       <c r="J5">
         <f t="shared" si="0"/>
         <v>8.611111111111111E-2</v>
       </c>
-      <c r="L5" s="11" t="s">
+      <c r="L5" s="10" t="s">
         <v>30</v>
       </c>
       <c r="M5">
@@ -40219,26 +40218,26 @@
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A6" s="9" t="s">
+      <c r="A6" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="B6" s="8">
+      <c r="B6">
         <v>3749</v>
       </c>
-      <c r="D6" s="9" t="s">
+      <c r="D6" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="E6" s="8">
+      <c r="E6">
         <v>409</v>
       </c>
-      <c r="I6" s="11" t="s">
+      <c r="I6" s="10" t="s">
         <v>23</v>
       </c>
       <c r="J6">
         <f t="shared" si="0"/>
         <v>0.10909575886903174</v>
       </c>
-      <c r="L6" s="11" t="s">
+      <c r="L6" s="10" t="s">
         <v>31</v>
       </c>
       <c r="M6">
@@ -40249,23 +40248,23 @@
       <c r="A7" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="B7" s="8">
+      <c r="B7">
         <v>1044</v>
       </c>
       <c r="D7" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="E7" s="8">
+      <c r="E7">
         <v>286</v>
       </c>
-      <c r="I7" s="10" t="s">
+      <c r="I7" s="9" t="s">
         <v>16</v>
       </c>
       <c r="J7">
         <f t="shared" si="0"/>
         <v>0.27394636015325668</v>
       </c>
-      <c r="L7" s="11" t="s">
+      <c r="L7" s="10" t="s">
         <v>32</v>
       </c>
       <c r="M7">
@@ -40273,19 +40272,19 @@
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A8" s="9" t="s">
+      <c r="A8" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="B8" s="8">
+      <c r="B8">
         <v>1020</v>
       </c>
-      <c r="D8" s="9" t="s">
+      <c r="D8" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="E8" s="8">
+      <c r="E8">
         <v>244</v>
       </c>
-      <c r="I8" s="11" t="s">
+      <c r="I8" s="10" t="s">
         <v>20</v>
       </c>
       <c r="J8">
@@ -40294,26 +40293,26 @@
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A9" s="9" t="s">
+      <c r="A9" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="B9" s="8">
+      <c r="B9">
         <v>24</v>
       </c>
-      <c r="D9" s="9" t="s">
+      <c r="D9" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="E9" s="8">
+      <c r="E9">
         <v>10</v>
       </c>
-      <c r="I9" s="11" t="s">
+      <c r="I9" s="10" t="s">
         <v>21</v>
       </c>
       <c r="J9">
         <f t="shared" si="0"/>
         <v>0.41666666666666669</v>
       </c>
-      <c r="L9" s="11" t="s">
+      <c r="L9" s="10" t="s">
         <v>33</v>
       </c>
     </row>
@@ -40321,21 +40320,21 @@
       <c r="A10" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="B10" s="8">
+      <c r="B10">
         <v>6393</v>
       </c>
-      <c r="D10" s="9" t="s">
+      <c r="D10" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="E10" s="8">
+      <c r="E10">
         <v>17</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="D11" s="9" t="s">
+      <c r="D11" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="E11" s="8">
+      <c r="E11">
         <v>15</v>
       </c>
     </row>
@@ -40343,39 +40342,39 @@
       <c r="D12" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="E12" s="8">
+      <c r="E12">
         <v>125</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="D13" s="9" t="s">
+      <c r="D13" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="E13" s="8">
+      <c r="E13">
         <v>57</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="D14" s="9" t="s">
+      <c r="D14" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="E14" s="8">
+      <c r="E14">
         <v>28</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="D15" s="9" t="s">
+      <c r="D15" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="E15" s="8">
+      <c r="E15">
         <v>25</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="D16" s="9" t="s">
+      <c r="D16" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="E16" s="8">
+      <c r="E16">
         <v>15</v>
       </c>
     </row>
@@ -40383,7 +40382,7 @@
       <c r="D17" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="E17" s="8">
+      <c r="E17">
         <v>9</v>
       </c>
     </row>
@@ -40391,7 +40390,7 @@
       <c r="D18" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="E18" s="8">
+      <c r="E18">
         <v>963</v>
       </c>
     </row>

</xml_diff>